<commit_message>
adding version metadata for evidence measurement method, evidence analysis method, interpretation method
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_validate_model.xlsx
+++ b/tests/fixtures/test_validate_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="989" activeTab="5"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="989" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="242">
   <si>
     <t>Table</t>
   </si>
@@ -444,438 +444,432 @@
     <t>Mass units</t>
   </si>
   <si>
-    <t>Volume distribution</t>
-  </si>
-  <si>
-    <t>Volume mean</t>
-  </si>
-  <si>
-    <t>Volume standard deviation</t>
-  </si>
-  <si>
-    <t>Volume units</t>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Units</t>
   </si>
   <si>
     <t>Initial density</t>
   </si>
   <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>normal_distribution</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular_compartment</t>
+  </si>
+  <si>
+    <t>density_e</t>
+  </si>
+  <si>
+    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>specie_1</t>
+  </si>
+  <si>
+    <t>specie_name_1</t>
+  </si>
+  <si>
+    <t>NaHCO</t>
+  </si>
+  <si>
+    <t>pseudo_species</t>
+  </si>
+  <si>
+    <t>specie_2</t>
+  </si>
+  <si>
+    <t>specie_name_2</t>
+  </si>
+  <si>
+    <t>N2O2P</t>
+  </si>
+  <si>
+    <t>specie_3</t>
+  </si>
+  <si>
+    <t>specie_name_3</t>
+  </si>
+  <si>
+    <t>N4O4P2</t>
+  </si>
+  <si>
+    <t>specie_4</t>
+  </si>
+  <si>
+    <t>specie_name_4</t>
+  </si>
+  <si>
+    <t>N10O10P5</t>
+  </si>
+  <si>
+    <t>specie_5</t>
+  </si>
+  <si>
+    <t>specie_name_5</t>
+  </si>
+  <si>
+    <t>N5O5</t>
+  </si>
+  <si>
+    <t>specie_6</t>
+  </si>
+  <si>
+    <t>specie_name_6</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Species type</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>specie_1[e]</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>specie_2[e]</t>
+  </si>
+  <si>
+    <t>specie_1[c]</t>
+  </si>
+  <si>
+    <t>specie_2[c]</t>
+  </si>
+  <si>
+    <t>specie_3[c]</t>
+  </si>
+  <si>
+    <t>specie_4[c]</t>
+  </si>
+  <si>
+    <t>specie_5[c]</t>
+  </si>
+  <si>
+    <t>specie_6[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_1[e]</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[e]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_4[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_5[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_6[c]</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>volume_c</t>
+  </si>
+  <si>
+    <t>c / density_c</t>
+  </si>
+  <si>
+    <t>volume_e</t>
+  </si>
+  <si>
+    <t>e / density_e</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Submodel</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Reversible</t>
+  </si>
+  <si>
+    <t>Rate units</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>reaction_1</t>
+  </si>
+  <si>
+    <t>reaction_name_1</t>
+  </si>
+  <si>
+    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>M s^-1</t>
+  </si>
+  <si>
+    <t>reaction_2</t>
+  </si>
+  <si>
+    <t>reaction_name_2</t>
+  </si>
+  <si>
+    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t>reaction_3</t>
+  </si>
+  <si>
+    <t>reaction_name_3</t>
+  </si>
+  <si>
+    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t>reaction_4</t>
+  </si>
+  <si>
+    <t>reaction_name_4</t>
+  </si>
+  <si>
+    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>reaction_1-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t>reaction_2-forward</t>
+  </si>
+  <si>
+    <t>k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>reaction_3-forward</t>
+  </si>
+  <si>
+    <t>k_cat_3_for * specie_4[c] / (specie_4[c] + k_m_3  * Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>reaction_3-backward</t>
+  </si>
+  <si>
+    <t>backward</t>
+  </si>
+  <si>
+    <t>k_cat_3_rev * (specie_5[c] + specie_6[c])</t>
+  </si>
+  <si>
+    <t>reaction_4-forward</t>
+  </si>
+  <si>
+    <t>k_cat_4 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>Reaction rate units</t>
+  </si>
+  <si>
+    <t>Coefficient units</t>
+  </si>
+  <si>
+    <t>dfba-obj-dfba_submodel</t>
+  </si>
+  <si>
+    <t>2*Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Cell size units</t>
+  </si>
+  <si>
+    <t>Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t>Metabolism net reaction</t>
+  </si>
+  <si>
+    <t>No comment</t>
+  </si>
+  <si>
+    <t>dFBA objective reaction</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_2[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 2</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_3[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 3</t>
+  </si>
+  <si>
+    <t>Standard error</t>
+  </si>
+  <si>
+    <t>fractionDryWeight</t>
+  </si>
+  <si>
+    <t>Fraction of cell mass which is non water</t>
+  </si>
+  <si>
+    <t>[Ref-0006]</t>
+  </si>
+  <si>
+    <t>k_cat_2</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>molecule^-1 s^-1</t>
+  </si>
+  <si>
+    <t>k_m_3</t>
+  </si>
+  <si>
+    <t>K_m</t>
+  </si>
+  <si>
+    <t>k_cat_1</t>
+  </si>
+  <si>
+    <t>k_cat_3_for</t>
+  </si>
+  <si>
+    <t>k_cat_3_rev</t>
+  </si>
+  <si>
+    <t>k_cat_4</t>
+  </si>
+  <si>
+    <t>g l^-1</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>molecule mol^-1</t>
+  </si>
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>Measurement method</t>
+  </si>
+  <si>
+    <t>Analysis method</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
     <t>pH units</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>cellular_compartment</t>
-  </si>
-  <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
-    <t>3D_compartment</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>normal_distribution</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>density_c</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>extracellular_compartment</t>
-  </si>
-  <si>
-    <t>density_e</t>
-  </si>
-  <si>
-    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>specie_1</t>
-  </si>
-  <si>
-    <t>specie_name_1</t>
-  </si>
-  <si>
-    <t>NaHCO</t>
-  </si>
-  <si>
-    <t>pseudo_species</t>
-  </si>
-  <si>
-    <t>specie_2</t>
-  </si>
-  <si>
-    <t>specie_name_2</t>
-  </si>
-  <si>
-    <t>N2O2P</t>
-  </si>
-  <si>
-    <t>specie_3</t>
-  </si>
-  <si>
-    <t>specie_name_3</t>
-  </si>
-  <si>
-    <t>N4O4P2</t>
-  </si>
-  <si>
-    <t>specie_4</t>
-  </si>
-  <si>
-    <t>specie_name_4</t>
-  </si>
-  <si>
-    <t>N10O10P5</t>
-  </si>
-  <si>
-    <t>specie_5</t>
-  </si>
-  <si>
-    <t>specie_name_5</t>
-  </si>
-  <si>
-    <t>N5O5</t>
-  </si>
-  <si>
-    <t>specie_6</t>
-  </si>
-  <si>
-    <t>specie_name_6</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>Species type</t>
-  </si>
-  <si>
-    <t>Compartment</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>specie_1[e]</t>
-  </si>
-  <si>
-    <t>molecule</t>
-  </si>
-  <si>
-    <t>specie_2[e]</t>
-  </si>
-  <si>
-    <t>specie_1[c]</t>
-  </si>
-  <si>
-    <t>specie_2[c]</t>
-  </si>
-  <si>
-    <t>specie_3[c]</t>
-  </si>
-  <si>
-    <t>specie_4[c]</t>
-  </si>
-  <si>
-    <t>specie_5[c]</t>
-  </si>
-  <si>
-    <t>specie_6[c]</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Standard deviation</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_1[e]</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[e]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_4[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_5[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_6[c]</t>
-  </si>
-  <si>
-    <t>Expression</t>
-  </si>
-  <si>
-    <t>volume_c</t>
-  </si>
-  <si>
-    <t>c / density_c</t>
-  </si>
-  <si>
-    <t>volume_e</t>
-  </si>
-  <si>
-    <t>e / density_e</t>
-  </si>
-  <si>
-    <t>Flux</t>
-  </si>
-  <si>
-    <t>Submodel</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Reversible</t>
-  </si>
-  <si>
-    <t>Rate units</t>
-  </si>
-  <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>reaction_1</t>
-  </si>
-  <si>
-    <t>reaction_name_1</t>
-  </si>
-  <si>
-    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t>s^-1</t>
-  </si>
-  <si>
-    <t>M s^-1</t>
-  </si>
-  <si>
-    <t>reaction_2</t>
-  </si>
-  <si>
-    <t>reaction_name_2</t>
-  </si>
-  <si>
-    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t>reaction_3</t>
-  </si>
-  <si>
-    <t>reaction_name_3</t>
-  </si>
-  <si>
-    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t>reaction_4</t>
-  </si>
-  <si>
-    <t>reaction_name_4</t>
-  </si>
-  <si>
-    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>reaction_1-forward</t>
-  </si>
-  <si>
-    <t>forward</t>
-  </si>
-  <si>
-    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t>reaction_2-forward</t>
-  </si>
-  <si>
-    <t>k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>reaction_3-forward</t>
-  </si>
-  <si>
-    <t>k_cat_3_for * specie_4[c] / (specie_4[c] + k_m_3  * Avogadro * volume_c)</t>
-  </si>
-  <si>
-    <t>reaction_3-backward</t>
-  </si>
-  <si>
-    <t>backward</t>
-  </si>
-  <si>
-    <t>k_cat_3_rev * (specie_5[c] + specie_6[c])</t>
-  </si>
-  <si>
-    <t>reaction_4-forward</t>
-  </si>
-  <si>
-    <t>k_cat_4 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Reaction rate units</t>
-  </si>
-  <si>
-    <t>Coefficient units</t>
-  </si>
-  <si>
-    <t>dfba-obj-dfba_submodel</t>
-  </si>
-  <si>
-    <t>2*Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Cell size units</t>
-  </si>
-  <si>
-    <t>Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t>Metabolism net reaction</t>
-  </si>
-  <si>
-    <t>No comment</t>
-  </si>
-  <si>
-    <t>dFBA objective reaction</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 1</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_2[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 2</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_3[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 3</t>
-  </si>
-  <si>
-    <t>Standard error</t>
-  </si>
-  <si>
-    <t>fractionDryWeight</t>
-  </si>
-  <si>
-    <t>Fraction of cell mass which is non water</t>
-  </si>
-  <si>
-    <t>[Ref-0006]</t>
-  </si>
-  <si>
-    <t>k_cat_2</t>
-  </si>
-  <si>
-    <t>k_cat</t>
-  </si>
-  <si>
-    <t>molecule^-1 s^-1</t>
-  </si>
-  <si>
-    <t>k_m_3</t>
-  </si>
-  <si>
-    <t>K_m</t>
-  </si>
-  <si>
-    <t>k_cat_1</t>
-  </si>
-  <si>
-    <t>k_cat_3_for</t>
-  </si>
-  <si>
-    <t>k_cat_3_rev</t>
-  </si>
-  <si>
-    <t>k_cat_4</t>
-  </si>
-  <si>
-    <t>g l^-1</t>
-  </si>
-  <si>
-    <t>Avogadro</t>
-  </si>
-  <si>
-    <t>molecule mol^-1</t>
-  </si>
-  <si>
-    <t>Genotype</t>
-  </si>
-  <si>
-    <t>Variant</t>
-  </si>
-  <si>
     <t>Growth media</t>
   </si>
   <si>
@@ -886,12 +880,6 @@
   </si>
   <si>
     <t>Experiment design</t>
-  </si>
-  <si>
-    <t>Measurement method</t>
-  </si>
-  <si>
-    <t>Analysis method</t>
   </si>
   <si>
     <t>Method</t>
@@ -986,11 +974,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="26">
@@ -1048,22 +1036,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1084,8 +1059,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1099,24 +1088,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1130,15 +1110,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1160,22 +1149,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1202,13 +1190,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,37 +1352,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1268,121 +1370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1402,6 +1390,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1444,6 +1447,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1461,184 +1484,149 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1657,6 +1645,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2109,216 +2100,216 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="3" width="15.7083333333333" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="23" hidden="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7083333333333" style="24" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="24" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26">
         <v>143</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26">
         <v>175</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26">
         <v>125</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26">
         <v>175</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26">
         <v>167</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26">
         <v>35</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26">
         <v>95</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:3">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26">
         <v>21</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2382,10 +2373,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
@@ -2437,8 +2428,8 @@
     <col min="8" max="8" width="10.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
     <col min="10" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333" style="19"/>
-    <col min="1027" max="16384" width="9" style="19"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="20"/>
+    <col min="1027" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
@@ -2449,10 +2440,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
@@ -2472,11 +2463,11 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>81</v>
@@ -2484,11 +2475,11 @@
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>81</v>
@@ -2532,11 +2523,11 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="G1" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -3564,25 +3555,25 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>40</v>
@@ -4615,22 +4606,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -4639,28 +4630,28 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N3" s="18"/>
+        <v>147</v>
+      </c>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1">
         <v>-1</v>
@@ -4669,48 +4660,48 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N4" s="18"/>
+        <v>147</v>
+      </c>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>160</v>
+      <c r="D6" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -4753,8 +4744,8 @@
     <col min="11" max="11" width="10.125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" style="1" customWidth="1"/>
     <col min="13" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333" style="15"/>
-    <col min="1027" max="16384" width="9" style="15"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="16"/>
+    <col min="1027" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
@@ -4765,19 +4756,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -4797,108 +4788,108 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="E2" s="12"/>
       <c r="F2" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="E3" s="12"/>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="E4" s="12"/>
       <c r="F4" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>167</v>
+      </c>
+      <c r="E5" s="12"/>
       <c r="F5" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="E6" s="12"/>
       <c r="F6" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4930,10 +4921,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
-      <c r="D1" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="14"/>
+      <c r="D1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -4943,19 +4934,19 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>40</v>
@@ -4975,22 +4966,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -5021,25 +5012,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="10" width="8.78333333333333" style="11"/>
+    <col min="1" max="10" width="8.78333333333333" style="12"/>
     <col min="11" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>181</v>
+      <c r="C1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -5050,31 +5041,31 @@
       <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A2" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>184</v>
+      <c r="I2" s="12" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -5099,32 +5090,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="2" width="8.78333333333333" style="11"/>
-    <col min="3" max="3" width="20.35" style="11"/>
-    <col min="4" max="10" width="8.78333333333333" style="11"/>
-    <col min="11" max="11" width="10.3916666666667" style="11"/>
+    <col min="1" max="2" width="8.78333333333333" style="12"/>
+    <col min="3" max="3" width="20.35" style="12"/>
+    <col min="4" max="10" width="8.78333333333333" style="12"/>
+    <col min="11" max="11" width="10.3916666666667" style="12"/>
     <col min="12" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333" style="10"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" ht="15.1" customHeight="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="11" customFormat="1" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>115</v>
+      <c r="E1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>40</v>
@@ -5135,80 +5126,80 @@
       <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A2" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>182</v>
       </c>
+      <c r="C2" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="13">
+        <v>118</v>
+      </c>
+      <c r="E2" s="14">
         <v>-3</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>151</v>
+      <c r="F2" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="11" t="s">
-        <v>188</v>
+      <c r="J2" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A3" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>182</v>
+      <c r="A3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="13">
+        <v>119</v>
+      </c>
+      <c r="E3" s="14">
         <v>-4</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>151</v>
+      <c r="F3" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A4" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>182</v>
+      <c r="A4" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="13">
+        <v>120</v>
+      </c>
+      <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>151</v>
+      <c r="F4" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -5241,7 +5232,7 @@
     <col min="3" max="3" width="18.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.25" style="1"/>
     <col min="5" max="1026" width="8.78333333333333" style="1"/>
-    <col min="1027" max="16384" width="9" style="8"/>
+    <col min="1027" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
@@ -5255,13 +5246,13 @@
         <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>40</v>
@@ -5281,112 +5272,112 @@
     </row>
     <row r="2" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="1" t="s">
         <v>83</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="8"/>
+        <v>192</v>
+      </c>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="9">
+        <v>193</v>
+      </c>
+      <c r="D3" s="10">
         <v>2000</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D4" s="9">
+        <v>196</v>
+      </c>
+      <c r="D4" s="10">
         <v>0.001</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" s="8"/>
+        <v>197</v>
+      </c>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="8"/>
+        <v>198</v>
+      </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>199</v>
+      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B8" s="8"/>
+        <v>200</v>
+      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
@@ -5397,7 +5388,7 @@
         <v>1100</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
@@ -5408,18 +5399,18 @@
         <v>1100</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D11" s="9">
+        <v>202</v>
+      </c>
+      <c r="D11" s="10">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5459,10 +5450,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
@@ -5493,37 +5484,45 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="2" width="13.3916666666667" style="1"/>
-    <col min="3" max="1033" width="9.10833333333333" style="1"/>
+    <col min="3" max="1035" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="7:14">
-      <c r="G1" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+    <row r="1" ht="15" customHeight="1" spans="7:20">
+      <c r="G1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:22">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="Q1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:24">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -5531,13 +5530,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>93</v>
@@ -5546,7 +5545,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>50</v>
@@ -5558,43 +5557,51 @@
         <v>61</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>72</v>
+        <v>208</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>214</v>
-      </c>
       <c r="Q2" s="5" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>216</v>
+        <v>29</v>
       </c>
       <c r="S2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:N1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -5718,65 +5725,70 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
-    <col min="3" max="1022" width="9.10833333333333" style="1"/>
-    <col min="1023" max="1023" width="9.10833333333333"/>
+    <col min="3" max="1023" width="9.10833333333333" style="1"/>
+    <col min="1024" max="1024" width="9.10833333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="7:8">
+      <c r="G1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="3:4">
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="3:4">
       <c r="C3" s="6"/>
@@ -5806,7 +5818,14 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
+    <row r="10" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -5842,46 +5861,46 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
@@ -5926,28 +5945,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -5991,25 +6010,25 @@
         <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -6030,7 +6049,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -6053,7 +6072,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1025" width="8.78333333333333" style="1"/>
-    <col min="1026" max="16384" width="9" style="8"/>
+    <col min="1026" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
@@ -6084,7 +6103,7 @@
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
@@ -6122,8 +6141,8 @@
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="1018" width="8.78333333333333" style="1"/>
-    <col min="1019" max="1019" width="8.78333333333333" style="22"/>
-    <col min="1020" max="16384" width="9" style="22"/>
+    <col min="1019" max="1019" width="8.78333333333333" style="23"/>
+    <col min="1020" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
@@ -6254,12 +6273,12 @@
   <sheetPr/>
   <dimension ref="A1:AMP4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
@@ -6278,17 +6297,17 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="14"/>
+      <c r="N1" s="15"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -7307,7 +7326,7 @@
       <c r="AMP1" s="3"/>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:1030">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -7344,10 +7363,10 @@
         <v>71</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>40</v>
@@ -8401,7 +8420,7 @@
       <c r="H3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="10">
         <v>4.58e-17</v>
       </c>
       <c r="J3" s="1">
@@ -8419,9 +8438,9 @@
       <c r="N3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="1" t="s">
         <v>84</v>
       </c>
@@ -8466,9 +8485,9 @@
       <c r="N4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
       <c r="R4" s="1" t="s">
         <v>88</v>
       </c>
@@ -8561,13 +8580,13 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -8585,13 +8604,13 @@
       <c r="F3" s="1">
         <v>-1</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -8609,13 +8628,13 @@
       <c r="F4" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
@@ -8633,13 +8652,13 @@
       <c r="F5" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="1" t="s">
@@ -8657,13 +8676,13 @@
       <c r="F6" s="1">
         <v>-3</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
@@ -8681,12 +8700,12 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L7">
@@ -8731,7 +8750,7 @@
         <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -8751,7 +8770,7 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>94</v>
@@ -8760,12 +8779,12 @@
         <v>78</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>98</v>
@@ -8774,12 +8793,12 @@
         <v>78</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>94</v>
@@ -8788,12 +8807,12 @@
         <v>73</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>98</v>
@@ -8802,12 +8821,12 @@
         <v>73</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>101</v>
@@ -8816,12 +8835,12 @@
         <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>104</v>
@@ -8830,12 +8849,12 @@
         <v>73</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>107</v>
@@ -8844,12 +8863,12 @@
         <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>110</v>
@@ -8858,7 +8877,7 @@
         <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -8900,16 +8919,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -8929,141 +8948,141 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="21">
         <v>0.000148</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="21">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="G2" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="21">
         <v>0.0002</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="21">
         <v>0.014142135623731</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="G3" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="21">
         <v>0.0005</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="21">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="G4" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="21">
         <v>0.0005</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="21">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="G5" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="21">
         <v>0.001</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
         <v>0.0316227766016838</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="G6" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="21">
         <v>0.002</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="21">
         <v>0.0447213595499958</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="G7" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>